<commit_message>
committed hello.txt and excelFile.xlsx
</commit_message>
<xml_diff>
--- a/excelFile.xlsx
+++ b/excelFile.xlsx
@@ -350,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -373,6 +373,16 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>